<commit_message>
Backup to GitHub - 2021.06.05
</commit_message>
<xml_diff>
--- a/01_Classification/03_Output/Back_Pain_00_Results_Summary.xlsx
+++ b/01_Classification/03_Output/Back_Pain_00_Results_Summary.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\DSML_Case_Studies\01_Classification\03_Output\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C5FFDEA-6920-42EC-AC03-E54A7339CF7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="27870" windowHeight="16440" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -15,7 +21,7 @@
     <sheet name="PCA_Top_Features" sheetId="6" r:id="rId6"/>
     <sheet name="DTR-Features" sheetId="7" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
@@ -166,8 +172,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -228,8 +234,94 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="11">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FF00B050"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -276,7 +368,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -308,9 +400,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -342,6 +452,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -517,14 +645,18 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -532,7 +664,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -543,7 +675,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -554,7 +686,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -565,7 +697,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -576,7 +708,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -587,7 +719,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -598,7 +730,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -609,7 +741,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -620,7 +752,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -631,7 +763,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -642,7 +774,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -653,7 +785,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -664,7 +796,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -681,14 +813,19 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:I14"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F12" sqref="F12"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="24.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>17</v>
       </c>
@@ -714,7 +851,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -725,7 +862,7 @@
         <v>60.497</v>
       </c>
       <c r="D2">
-        <v>17.237</v>
+        <v>17.236999999999998</v>
       </c>
       <c r="E2">
         <v>26.148</v>
@@ -734,7 +871,7 @@
         <v>46.43</v>
       </c>
       <c r="G2">
-        <v>58.691</v>
+        <v>58.691000000000003</v>
       </c>
       <c r="H2">
         <v>72.878</v>
@@ -743,7 +880,7 @@
         <v>129.834</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -751,28 +888,28 @@
         <v>310</v>
       </c>
       <c r="C3">
-        <v>17.543</v>
+        <v>17.542999999999999</v>
       </c>
       <c r="D3">
-        <v>10.008</v>
+        <v>10.007999999999999</v>
       </c>
       <c r="E3">
-        <v>-6.555</v>
+        <v>-6.5549999999999997</v>
       </c>
       <c r="F3">
         <v>10.667</v>
       </c>
       <c r="G3">
-        <v>16.358</v>
+        <v>16.358000000000001</v>
       </c>
       <c r="H3">
         <v>22.12</v>
       </c>
       <c r="I3">
-        <v>49.432</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9">
+        <v>49.432000000000002</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
@@ -780,10 +917,10 @@
         <v>310</v>
       </c>
       <c r="C4">
-        <v>51.931</v>
+        <v>51.930999999999997</v>
       </c>
       <c r="D4">
-        <v>18.554</v>
+        <v>18.553999999999998</v>
       </c>
       <c r="E4">
         <v>14</v>
@@ -792,7 +929,7 @@
         <v>37</v>
       </c>
       <c r="G4">
-        <v>49.562</v>
+        <v>49.561999999999998</v>
       </c>
       <c r="H4">
         <v>63</v>
@@ -801,7 +938,7 @@
         <v>125.742</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
@@ -809,28 +946,28 @@
         <v>310</v>
       </c>
       <c r="C5">
-        <v>42.954</v>
+        <v>42.954000000000001</v>
       </c>
       <c r="D5">
         <v>13.423</v>
       </c>
       <c r="E5">
-        <v>13.367</v>
+        <v>13.367000000000001</v>
       </c>
       <c r="F5">
-        <v>33.347</v>
+        <v>33.347000000000001</v>
       </c>
       <c r="G5">
-        <v>42.405</v>
+        <v>42.405000000000001</v>
       </c>
       <c r="H5">
-        <v>52.696</v>
+        <v>52.695999999999998</v>
       </c>
       <c r="I5">
         <v>121.43</v>
       </c>
     </row>
-    <row r="6" spans="1:9">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
@@ -838,13 +975,13 @@
         <v>310</v>
       </c>
       <c r="C6">
-        <v>117.921</v>
+        <v>117.92100000000001</v>
       </c>
       <c r="D6">
         <v>13.317</v>
       </c>
       <c r="E6">
-        <v>70.083</v>
+        <v>70.082999999999998</v>
       </c>
       <c r="F6">
         <v>110.709</v>
@@ -859,7 +996,7 @@
         <v>163.071</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -867,28 +1004,28 @@
         <v>310</v>
       </c>
       <c r="C7">
-        <v>26.297</v>
+        <v>26.297000000000001</v>
       </c>
       <c r="D7">
-        <v>37.559</v>
+        <v>37.558999999999997</v>
       </c>
       <c r="E7">
         <v>-11.058</v>
       </c>
       <c r="F7">
-        <v>1.604</v>
+        <v>1.6040000000000001</v>
       </c>
       <c r="G7">
-        <v>11.768</v>
+        <v>11.768000000000001</v>
       </c>
       <c r="H7">
-        <v>41.287</v>
+        <v>41.286999999999999</v>
       </c>
       <c r="I7">
-        <v>418.543</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9">
+        <v>418.54300000000001</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
         <v>8</v>
       </c>
@@ -896,28 +1033,28 @@
         <v>310</v>
       </c>
       <c r="C8">
-        <v>0.473</v>
+        <v>0.47299999999999998</v>
       </c>
       <c r="D8">
-        <v>0.286</v>
+        <v>0.28599999999999998</v>
       </c>
       <c r="E8">
-        <v>0.003</v>
+        <v>3.0000000000000001E-3</v>
       </c>
       <c r="F8">
         <v>0.224</v>
       </c>
       <c r="G8">
-        <v>0.476</v>
+        <v>0.47599999999999998</v>
       </c>
       <c r="H8">
-        <v>0.705</v>
+        <v>0.70499999999999996</v>
       </c>
       <c r="I8">
         <v>0.999</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
         <v>9</v>
       </c>
@@ -925,13 +1062,13 @@
         <v>310</v>
       </c>
       <c r="C9">
-        <v>21.322</v>
+        <v>21.321999999999999</v>
       </c>
       <c r="D9">
-        <v>8.638999999999999</v>
+        <v>8.6389999999999993</v>
       </c>
       <c r="E9">
-        <v>7.027</v>
+        <v>7.0270000000000001</v>
       </c>
       <c r="F9">
         <v>13.054</v>
@@ -940,13 +1077,13 @@
         <v>21.907</v>
       </c>
       <c r="H9">
-        <v>28.954</v>
+        <v>28.954000000000001</v>
       </c>
       <c r="I9">
         <v>36.744</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
         <v>10</v>
       </c>
@@ -960,22 +1097,22 @@
         <v>3.4</v>
       </c>
       <c r="E10">
-        <v>7.038</v>
+        <v>7.0380000000000003</v>
       </c>
       <c r="F10">
-        <v>10.418</v>
+        <v>10.417999999999999</v>
       </c>
       <c r="G10">
-        <v>12.938</v>
+        <v>12.938000000000001</v>
       </c>
       <c r="H10">
         <v>15.89</v>
       </c>
       <c r="I10">
-        <v>19.324</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9">
+        <v>19.324000000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
         <v>11</v>
       </c>
@@ -986,25 +1123,25 @@
         <v>11.933</v>
       </c>
       <c r="D11">
-        <v>2.893</v>
+        <v>2.8929999999999998</v>
       </c>
       <c r="E11">
-        <v>7.031</v>
+        <v>7.0309999999999997</v>
       </c>
       <c r="F11">
-        <v>9.541</v>
+        <v>9.5410000000000004</v>
       </c>
       <c r="G11">
-        <v>11.954</v>
+        <v>11.954000000000001</v>
       </c>
       <c r="H11">
         <v>14.372</v>
       </c>
       <c r="I11">
-        <v>16.821</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9">
+        <v>16.821000000000002</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
         <v>12</v>
       </c>
@@ -1012,28 +1149,28 @@
         <v>310</v>
       </c>
       <c r="C12">
-        <v>-14.053</v>
+        <v>-14.053000000000001</v>
       </c>
       <c r="D12">
-        <v>12.226</v>
+        <v>12.226000000000001</v>
       </c>
       <c r="E12">
-        <v>-35.287</v>
+        <v>-35.286999999999999</v>
       </c>
       <c r="F12">
         <v>-24.29</v>
       </c>
       <c r="G12">
-        <v>-14.623</v>
+        <v>-14.622999999999999</v>
       </c>
       <c r="H12">
-        <v>-3.497</v>
+        <v>-3.4969999999999999</v>
       </c>
       <c r="I12">
-        <v>6.972</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9">
+        <v>6.9720000000000004</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
         <v>13</v>
       </c>
@@ -1041,10 +1178,10 @@
         <v>310</v>
       </c>
       <c r="C13">
-        <v>25.646</v>
+        <v>25.646000000000001</v>
       </c>
       <c r="D13">
-        <v>10.451</v>
+        <v>10.451000000000001</v>
       </c>
       <c r="E13">
         <v>7.008</v>
@@ -1053,16 +1190,16 @@
         <v>17.189</v>
       </c>
       <c r="G13">
-        <v>24.932</v>
+        <v>24.931999999999999</v>
       </c>
       <c r="H13">
-        <v>33.98</v>
+        <v>33.979999999999997</v>
       </c>
       <c r="I13">
-        <v>44.341</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9">
+        <v>44.341000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
         <v>14</v>
       </c>
@@ -1070,10 +1207,10 @@
         <v>310</v>
       </c>
       <c r="C14">
-        <v>0.677</v>
+        <v>0.67700000000000005</v>
       </c>
       <c r="D14">
-        <v>0.468</v>
+        <v>0.46800000000000003</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -1097,14 +1234,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:C14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>25</v>
       </c>
@@ -1112,7 +1249,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1120,10 +1257,10 @@
         <v>2</v>
       </c>
       <c r="C2">
-        <v>1702684169138.184</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>1702684169138.1841</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1131,10 +1268,10 @@
         <v>3</v>
       </c>
       <c r="C3">
-        <v>175445553180.6422</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3">
+        <v>175445553180.64221</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1142,10 +1279,10 @@
         <v>4</v>
       </c>
       <c r="C4">
-        <v>19.50774117993969</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>19.507741179939689</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1153,10 +1290,10 @@
         <v>5</v>
       </c>
       <c r="C5">
-        <v>871439556379.74</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>871439556379.73999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1167,7 +1304,7 @@
         <v>35.30375091396494</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1175,10 +1312,10 @@
         <v>7</v>
       </c>
       <c r="C7">
-        <v>2.663584692152483</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>2.6635846921524831</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1189,7 +1326,7 @@
         <v>3.833090484865858</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1197,10 +1334,10 @@
         <v>9</v>
       </c>
       <c r="C9">
-        <v>7.281564651749722</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>7.2815646517497221</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1208,10 +1345,10 @@
         <v>10</v>
       </c>
       <c r="C10">
-        <v>15.25995404286084</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>15.259954042860841</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1219,10 +1356,10 @@
         <v>11</v>
       </c>
       <c r="C11">
-        <v>17.32643228856763</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>17.326432288567631</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1233,7 +1370,7 @@
         <v>2.319777720456794</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1241,10 +1378,10 @@
         <v>13</v>
       </c>
       <c r="C13">
-        <v>6.989135309972847</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3">
+        <v>6.9891353099728466</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1261,27 +1398,27 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:B11"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B1" s="1">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:2">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>0.273</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>0.27300000000000002</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1289,68 +1426,68 @@
         <v>0.104</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>0.095</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>9.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.08799999999999999</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>8.7999999999999995E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.08500000000000001</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
+        <v>8.5000000000000006E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>0.081</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
+        <v>8.1000000000000003E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>0.074</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
+        <v>7.3999999999999996E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0.074</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2">
+        <v>7.3999999999999996E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>0.061</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2">
+        <v>6.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>0.039</v>
+        <v>3.9E-2</v>
       </c>
     </row>
   </sheetData>
@@ -1359,14 +1496,16 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:M11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+  <dimension ref="A1:Z11"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="P19" sqref="P19"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:13">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.25">
       <c r="B1" s="1">
         <v>0</v>
       </c>
@@ -1404,7 +1543,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1412,54 +1551,102 @@
         <v>0.53</v>
       </c>
       <c r="C2">
-        <v>0.322</v>
+        <v>0.32200000000000001</v>
       </c>
       <c r="D2">
-        <v>0.456</v>
+        <v>0.45600000000000002</v>
       </c>
       <c r="E2">
         <v>0.441</v>
       </c>
       <c r="F2">
-        <v>-0.144</v>
+        <v>-0.14399999999999999</v>
       </c>
       <c r="G2">
-        <v>0.421</v>
+        <v>0.42099999999999999</v>
       </c>
       <c r="H2">
-        <v>0.044</v>
+        <v>4.3999999999999997E-2</v>
       </c>
       <c r="I2">
-        <v>-0.075</v>
+        <v>-7.4999999999999997E-2</v>
       </c>
       <c r="J2">
-        <v>-0.07000000000000001</v>
+        <v>-7.0000000000000007E-2</v>
       </c>
       <c r="K2">
-        <v>0.032</v>
+        <v>3.2000000000000001E-2</v>
       </c>
       <c r="L2">
-        <v>0.026</v>
+        <v>2.5999999999999999E-2</v>
       </c>
       <c r="M2">
-        <v>-0.019</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13">
+        <v>-1.9E-2</v>
+      </c>
+      <c r="O2">
+        <f>ABS(B2)</f>
+        <v>0.53</v>
+      </c>
+      <c r="P2">
+        <f t="shared" ref="P2:Z2" si="0">ABS(C2)</f>
+        <v>0.32200000000000001</v>
+      </c>
+      <c r="Q2">
+        <f t="shared" si="0"/>
+        <v>0.45600000000000002</v>
+      </c>
+      <c r="R2">
+        <f t="shared" si="0"/>
+        <v>0.441</v>
+      </c>
+      <c r="S2">
+        <f t="shared" si="0"/>
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="T2">
+        <f t="shared" si="0"/>
+        <v>0.42099999999999999</v>
+      </c>
+      <c r="U2">
+        <f t="shared" si="0"/>
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="V2">
+        <f t="shared" si="0"/>
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="W2">
+        <f t="shared" si="0"/>
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="X2">
+        <f t="shared" si="0"/>
+        <v>3.2000000000000001E-2</v>
+      </c>
+      <c r="Y2">
+        <f t="shared" si="0"/>
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="Z2">
+        <f t="shared" si="0"/>
+        <v>1.9E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>-0.025</v>
+        <v>-2.5000000000000001E-2</v>
       </c>
       <c r="C3">
-        <v>0.415</v>
+        <v>0.41499999999999998</v>
       </c>
       <c r="D3">
-        <v>0.08599999999999999</v>
+        <v>8.5999999999999993E-2</v>
       </c>
       <c r="E3">
-        <v>-0.342</v>
+        <v>-0.34200000000000003</v>
       </c>
       <c r="F3">
         <v>0.623</v>
@@ -1468,7 +1655,7 @@
         <v>0.157</v>
       </c>
       <c r="H3">
-        <v>0.269</v>
+        <v>0.26900000000000002</v>
       </c>
       <c r="I3">
         <v>0.1</v>
@@ -1485,254 +1672,590 @@
       <c r="M3">
         <v>-0.315</v>
       </c>
-    </row>
-    <row r="4" spans="1:13">
+      <c r="O3">
+        <f t="shared" ref="O3:O11" si="1">ABS(B3)</f>
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="P3">
+        <f t="shared" ref="P3:P11" si="2">ABS(C3)</f>
+        <v>0.41499999999999998</v>
+      </c>
+      <c r="Q3">
+        <f t="shared" ref="Q3:Q11" si="3">ABS(D3)</f>
+        <v>8.5999999999999993E-2</v>
+      </c>
+      <c r="R3">
+        <f t="shared" ref="R3:R11" si="4">ABS(E3)</f>
+        <v>0.34200000000000003</v>
+      </c>
+      <c r="S3">
+        <f t="shared" ref="S3:S11" si="5">ABS(F3)</f>
+        <v>0.623</v>
+      </c>
+      <c r="T3">
+        <f t="shared" ref="T3:T11" si="6">ABS(G3)</f>
+        <v>0.157</v>
+      </c>
+      <c r="U3">
+        <f t="shared" ref="U3:U11" si="7">ABS(H3)</f>
+        <v>0.26900000000000002</v>
+      </c>
+      <c r="V3">
+        <f t="shared" ref="V3:V11" si="8">ABS(I3)</f>
+        <v>0.1</v>
+      </c>
+      <c r="W3">
+        <f t="shared" ref="W3:W11" si="9">ABS(J3)</f>
+        <v>0.121</v>
+      </c>
+      <c r="X3">
+        <f t="shared" ref="X3:X11" si="10">ABS(K3)</f>
+        <v>0.187</v>
+      </c>
+      <c r="Y3">
+        <f t="shared" ref="Y3:Y11" si="11">ABS(L3)</f>
+        <v>0.245</v>
+      </c>
+      <c r="Z3">
+        <f t="shared" ref="Z3:Z11" si="12">ABS(M3)</f>
+        <v>0.315</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>-0.029</v>
+        <v>-2.9000000000000001E-2</v>
       </c>
       <c r="C4">
-        <v>-0.28</v>
+        <v>-0.28000000000000003</v>
       </c>
       <c r="D4">
         <v>-0.03</v>
       </c>
       <c r="E4">
-        <v>0.171</v>
+        <v>0.17100000000000001</v>
       </c>
       <c r="F4">
-        <v>-0.265</v>
+        <v>-0.26500000000000001</v>
       </c>
       <c r="G4">
-        <v>-0.008</v>
+        <v>-8.0000000000000002E-3</v>
       </c>
       <c r="H4">
-        <v>0.468</v>
+        <v>0.46800000000000003</v>
       </c>
       <c r="I4">
         <v>0.308</v>
       </c>
       <c r="J4">
-        <v>0.203</v>
+        <v>0.20300000000000001</v>
       </c>
       <c r="K4">
         <v>0.629</v>
       </c>
       <c r="L4">
-        <v>0.257</v>
+        <v>0.25700000000000001</v>
       </c>
       <c r="M4">
-        <v>0.061</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="O4">
+        <f t="shared" si="1"/>
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="P4">
+        <f t="shared" si="2"/>
+        <v>0.28000000000000003</v>
+      </c>
+      <c r="Q4">
+        <f t="shared" si="3"/>
+        <v>0.03</v>
+      </c>
+      <c r="R4">
+        <f t="shared" si="4"/>
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="S4">
+        <f t="shared" si="5"/>
+        <v>0.26500000000000001</v>
+      </c>
+      <c r="T4">
+        <f t="shared" si="6"/>
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="U4">
+        <f t="shared" si="7"/>
+        <v>0.46800000000000003</v>
+      </c>
+      <c r="V4">
+        <f t="shared" si="8"/>
+        <v>0.308</v>
+      </c>
+      <c r="W4">
+        <f t="shared" si="9"/>
+        <v>0.20300000000000001</v>
+      </c>
+      <c r="X4">
+        <f t="shared" si="10"/>
+        <v>0.629</v>
+      </c>
+      <c r="Y4">
+        <f t="shared" si="11"/>
+        <v>0.25700000000000001</v>
+      </c>
+      <c r="Z4">
+        <f t="shared" si="12"/>
+        <v>6.0999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>0.008</v>
+        <v>8.0000000000000002E-3</v>
       </c>
       <c r="C5">
-        <v>-0.073</v>
+        <v>-7.2999999999999995E-2</v>
       </c>
       <c r="D5">
-        <v>-0.048</v>
+        <v>-4.8000000000000001E-2</v>
       </c>
       <c r="E5">
-        <v>0.065</v>
+        <v>6.5000000000000002E-2</v>
       </c>
       <c r="F5">
-        <v>-0.076</v>
+        <v>-7.5999999999999998E-2</v>
       </c>
       <c r="G5">
-        <v>0.021</v>
+        <v>2.1000000000000001E-2</v>
       </c>
       <c r="H5">
-        <v>0.232</v>
+        <v>0.23200000000000001</v>
       </c>
       <c r="I5">
-        <v>0.462</v>
+        <v>0.46200000000000002</v>
       </c>
       <c r="J5">
-        <v>-0.332</v>
+        <v>-0.33200000000000002</v>
       </c>
       <c r="K5">
         <v>-0.109</v>
       </c>
       <c r="L5">
-        <v>-0.517</v>
+        <v>-0.51700000000000002</v>
       </c>
       <c r="M5">
-        <v>-0.57</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13">
+        <v>-0.56999999999999995</v>
+      </c>
+      <c r="O5">
+        <f t="shared" si="1"/>
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="P5">
+        <f t="shared" si="2"/>
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="Q5">
+        <f t="shared" si="3"/>
+        <v>4.8000000000000001E-2</v>
+      </c>
+      <c r="R5">
+        <f t="shared" si="4"/>
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="S5">
+        <f t="shared" si="5"/>
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="T5">
+        <f t="shared" si="6"/>
+        <v>2.1000000000000001E-2</v>
+      </c>
+      <c r="U5">
+        <f t="shared" si="7"/>
+        <v>0.23200000000000001</v>
+      </c>
+      <c r="V5">
+        <f t="shared" si="8"/>
+        <v>0.46200000000000002</v>
+      </c>
+      <c r="W5">
+        <f t="shared" si="9"/>
+        <v>0.33200000000000002</v>
+      </c>
+      <c r="X5">
+        <f t="shared" si="10"/>
+        <v>0.109</v>
+      </c>
+      <c r="Y5">
+        <f t="shared" si="11"/>
+        <v>0.51700000000000002</v>
+      </c>
+      <c r="Z5">
+        <f t="shared" si="12"/>
+        <v>0.56999999999999995</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>0.066</v>
+        <v>6.6000000000000003E-2</v>
       </c>
       <c r="C6">
-        <v>0.118</v>
+        <v>0.11799999999999999</v>
       </c>
       <c r="D6">
-        <v>0.041</v>
+        <v>4.1000000000000002E-2</v>
       </c>
       <c r="E6">
-        <v>-0.003</v>
+        <v>-3.0000000000000001E-3</v>
       </c>
       <c r="F6">
-        <v>0.168</v>
+        <v>0.16800000000000001</v>
       </c>
       <c r="G6">
-        <v>0.07099999999999999</v>
+        <v>7.0999999999999994E-2</v>
       </c>
       <c r="H6">
-        <v>-0.452</v>
+        <v>-0.45200000000000001</v>
       </c>
       <c r="I6">
         <v>0.504</v>
       </c>
       <c r="J6">
-        <v>0.429</v>
+        <v>0.42899999999999999</v>
       </c>
       <c r="K6">
-        <v>0.227</v>
+        <v>0.22700000000000001</v>
       </c>
       <c r="L6">
-        <v>-0.421</v>
+        <v>-0.42099999999999999</v>
       </c>
       <c r="M6">
-        <v>0.275</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13">
+        <v>0.27500000000000002</v>
+      </c>
+      <c r="O6">
+        <f t="shared" si="1"/>
+        <v>6.6000000000000003E-2</v>
+      </c>
+      <c r="P6">
+        <f t="shared" si="2"/>
+        <v>0.11799999999999999</v>
+      </c>
+      <c r="Q6">
+        <f t="shared" si="3"/>
+        <v>4.1000000000000002E-2</v>
+      </c>
+      <c r="R6">
+        <f t="shared" si="4"/>
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="S6">
+        <f t="shared" si="5"/>
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="T6">
+        <f t="shared" si="6"/>
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="U6">
+        <f t="shared" si="7"/>
+        <v>0.45200000000000001</v>
+      </c>
+      <c r="V6">
+        <f t="shared" si="8"/>
+        <v>0.504</v>
+      </c>
+      <c r="W6">
+        <f t="shared" si="9"/>
+        <v>0.42899999999999999</v>
+      </c>
+      <c r="X6">
+        <f t="shared" si="10"/>
+        <v>0.22700000000000001</v>
+      </c>
+      <c r="Y6">
+        <f t="shared" si="11"/>
+        <v>0.42099999999999999</v>
+      </c>
+      <c r="Z6">
+        <f t="shared" si="12"/>
+        <v>0.27500000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>-0.006</v>
+        <v>-6.0000000000000001E-3</v>
       </c>
       <c r="C7">
         <v>-0.13</v>
       </c>
       <c r="D7">
-        <v>0.027</v>
+        <v>2.7E-2</v>
       </c>
       <c r="E7">
-        <v>0.089</v>
+        <v>8.8999999999999996E-2</v>
       </c>
       <c r="F7">
         <v>-0.106</v>
       </c>
       <c r="G7">
-        <v>0.006</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="H7">
-        <v>0.097</v>
+        <v>9.7000000000000003E-2</v>
       </c>
       <c r="I7">
-        <v>-0.349</v>
+        <v>-0.34899999999999998</v>
       </c>
       <c r="J7">
-        <v>0.759</v>
+        <v>0.75900000000000001</v>
       </c>
       <c r="K7">
         <v>-0.15</v>
       </c>
       <c r="L7">
-        <v>-0.194</v>
+        <v>-0.19400000000000001</v>
       </c>
       <c r="M7">
         <v>-0.442</v>
       </c>
-    </row>
-    <row r="8" spans="1:13">
+      <c r="O7">
+        <f t="shared" si="1"/>
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="P7">
+        <f t="shared" si="2"/>
+        <v>0.13</v>
+      </c>
+      <c r="Q7">
+        <f t="shared" si="3"/>
+        <v>2.7E-2</v>
+      </c>
+      <c r="R7">
+        <f t="shared" si="4"/>
+        <v>8.8999999999999996E-2</v>
+      </c>
+      <c r="S7">
+        <f t="shared" si="5"/>
+        <v>0.106</v>
+      </c>
+      <c r="T7">
+        <f t="shared" si="6"/>
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="U7">
+        <f t="shared" si="7"/>
+        <v>9.7000000000000003E-2</v>
+      </c>
+      <c r="V7">
+        <f t="shared" si="8"/>
+        <v>0.34899999999999998</v>
+      </c>
+      <c r="W7">
+        <f t="shared" si="9"/>
+        <v>0.75900000000000001</v>
+      </c>
+      <c r="X7">
+        <f t="shared" si="10"/>
+        <v>0.15</v>
+      </c>
+      <c r="Y7">
+        <f t="shared" si="11"/>
+        <v>0.19400000000000001</v>
+      </c>
+      <c r="Z7">
+        <f t="shared" si="12"/>
+        <v>0.442</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>-0.035</v>
+        <v>-3.5000000000000003E-2</v>
       </c>
       <c r="C8">
-        <v>0.165</v>
+        <v>0.16500000000000001</v>
       </c>
       <c r="D8">
-        <v>-0.037</v>
+        <v>-3.6999999999999998E-2</v>
       </c>
       <c r="E8">
-        <v>-0.168</v>
+        <v>-0.16800000000000001</v>
       </c>
       <c r="F8">
-        <v>0.017</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="G8">
-        <v>0.017</v>
+        <v>1.7000000000000001E-2</v>
       </c>
       <c r="H8">
-        <v>0.304</v>
+        <v>0.30399999999999999</v>
       </c>
       <c r="I8">
-        <v>-0.481</v>
+        <v>-0.48099999999999998</v>
       </c>
       <c r="J8">
-        <v>-0.138</v>
+        <v>-0.13800000000000001</v>
       </c>
       <c r="K8">
-        <v>0.402</v>
+        <v>0.40200000000000002</v>
       </c>
       <c r="L8">
-        <v>-0.611</v>
+        <v>-0.61099999999999999</v>
       </c>
       <c r="M8">
         <v>0.253</v>
       </c>
-    </row>
-    <row r="9" spans="1:13">
+      <c r="O8">
+        <f t="shared" si="1"/>
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="P8">
+        <f t="shared" si="2"/>
+        <v>0.16500000000000001</v>
+      </c>
+      <c r="Q8">
+        <f t="shared" si="3"/>
+        <v>3.6999999999999998E-2</v>
+      </c>
+      <c r="R8">
+        <f t="shared" si="4"/>
+        <v>0.16800000000000001</v>
+      </c>
+      <c r="S8">
+        <f t="shared" si="5"/>
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="T8">
+        <f t="shared" si="6"/>
+        <v>1.7000000000000001E-2</v>
+      </c>
+      <c r="U8">
+        <f t="shared" si="7"/>
+        <v>0.30399999999999999</v>
+      </c>
+      <c r="V8">
+        <f t="shared" si="8"/>
+        <v>0.48099999999999998</v>
+      </c>
+      <c r="W8">
+        <f t="shared" si="9"/>
+        <v>0.13800000000000001</v>
+      </c>
+      <c r="X8">
+        <f t="shared" si="10"/>
+        <v>0.40200000000000002</v>
+      </c>
+      <c r="Y8">
+        <f t="shared" si="11"/>
+        <v>0.61099999999999999</v>
+      </c>
+      <c r="Z8">
+        <f t="shared" si="12"/>
+        <v>0.253</v>
+      </c>
+    </row>
+    <row r="9" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>0.016</v>
+        <v>1.6E-2</v>
       </c>
       <c r="C9">
         <v>-0.186</v>
       </c>
       <c r="D9">
-        <v>-0.008</v>
+        <v>-8.0000000000000002E-3</v>
       </c>
       <c r="E9">
         <v>0.159</v>
       </c>
       <c r="F9">
-        <v>0.325</v>
+        <v>0.32500000000000001</v>
       </c>
       <c r="G9">
-        <v>0.137</v>
+        <v>0.13700000000000001</v>
       </c>
       <c r="H9">
-        <v>0.535</v>
+        <v>0.53500000000000003</v>
       </c>
       <c r="I9">
         <v>0.157</v>
       </c>
       <c r="J9">
-        <v>0.14</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="K9">
-        <v>-0.506</v>
+        <v>-0.50600000000000001</v>
       </c>
       <c r="L9">
         <v>-0.111</v>
       </c>
       <c r="M9">
-        <v>0.465</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13">
+        <v>0.46500000000000002</v>
+      </c>
+      <c r="O9">
+        <f t="shared" si="1"/>
+        <v>1.6E-2</v>
+      </c>
+      <c r="P9">
+        <f t="shared" si="2"/>
+        <v>0.186</v>
+      </c>
+      <c r="Q9">
+        <f t="shared" si="3"/>
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="R9">
+        <f t="shared" si="4"/>
+        <v>0.159</v>
+      </c>
+      <c r="S9">
+        <f t="shared" si="5"/>
+        <v>0.32500000000000001</v>
+      </c>
+      <c r="T9">
+        <f t="shared" si="6"/>
+        <v>0.13700000000000001</v>
+      </c>
+      <c r="U9">
+        <f t="shared" si="7"/>
+        <v>0.53500000000000003</v>
+      </c>
+      <c r="V9">
+        <f t="shared" si="8"/>
+        <v>0.157</v>
+      </c>
+      <c r="W9">
+        <f t="shared" si="9"/>
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="X9">
+        <f t="shared" si="10"/>
+        <v>0.50600000000000001</v>
+      </c>
+      <c r="Y9">
+        <f t="shared" si="11"/>
+        <v>0.111</v>
+      </c>
+      <c r="Z9">
+        <f t="shared" si="12"/>
+        <v>0.46500000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1740,40 +2263,88 @@
         <v>-0.125</v>
       </c>
       <c r="C10">
-        <v>-0.598</v>
+        <v>-0.59799999999999998</v>
       </c>
       <c r="D10">
         <v>0.184</v>
       </c>
       <c r="E10">
-        <v>0.285</v>
+        <v>0.28499999999999998</v>
       </c>
       <c r="F10">
-        <v>0.514</v>
+        <v>0.51400000000000001</v>
       </c>
       <c r="G10">
-        <v>0.231</v>
+        <v>0.23100000000000001</v>
       </c>
       <c r="H10">
-        <v>-0.232</v>
+        <v>-0.23200000000000001</v>
       </c>
       <c r="I10">
-        <v>-0.196</v>
+        <v>-0.19600000000000001</v>
       </c>
       <c r="J10">
-        <v>-0.173</v>
+        <v>-0.17299999999999999</v>
       </c>
       <c r="K10">
-        <v>0.234</v>
+        <v>0.23400000000000001</v>
       </c>
       <c r="L10">
-        <v>-0.044</v>
+        <v>-4.3999999999999997E-2</v>
       </c>
       <c r="M10">
         <v>-0.127</v>
       </c>
-    </row>
-    <row r="11" spans="1:13">
+      <c r="O10">
+        <f t="shared" si="1"/>
+        <v>0.125</v>
+      </c>
+      <c r="P10">
+        <f t="shared" si="2"/>
+        <v>0.59799999999999998</v>
+      </c>
+      <c r="Q10">
+        <f t="shared" si="3"/>
+        <v>0.184</v>
+      </c>
+      <c r="R10">
+        <f t="shared" si="4"/>
+        <v>0.28499999999999998</v>
+      </c>
+      <c r="S10">
+        <f t="shared" si="5"/>
+        <v>0.51400000000000001</v>
+      </c>
+      <c r="T10">
+        <f t="shared" si="6"/>
+        <v>0.23100000000000001</v>
+      </c>
+      <c r="U10">
+        <f t="shared" si="7"/>
+        <v>0.23200000000000001</v>
+      </c>
+      <c r="V10">
+        <f t="shared" si="8"/>
+        <v>0.19600000000000001</v>
+      </c>
+      <c r="W10">
+        <f t="shared" si="9"/>
+        <v>0.17299999999999999</v>
+      </c>
+      <c r="X10">
+        <f t="shared" si="10"/>
+        <v>0.23400000000000001</v>
+      </c>
+      <c r="Y10">
+        <f t="shared" si="11"/>
+        <v>4.3999999999999997E-2</v>
+      </c>
+      <c r="Z10">
+        <f t="shared" si="12"/>
+        <v>0.127</v>
+      </c>
+    </row>
+    <row r="11" spans="1:26" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1781,53 +2352,161 @@
         <v>-0.106</v>
       </c>
       <c r="C11">
-        <v>-0.016</v>
+        <v>-1.6E-2</v>
       </c>
       <c r="D11">
-        <v>-0.538</v>
+        <v>-0.53800000000000003</v>
       </c>
       <c r="E11">
         <v>-0.125</v>
       </c>
       <c r="F11">
-        <v>-0.171</v>
+        <v>-0.17100000000000001</v>
       </c>
       <c r="G11">
-        <v>0.803</v>
+        <v>0.80300000000000005</v>
       </c>
       <c r="H11">
-        <v>-0.077</v>
+        <v>-7.6999999999999999E-2</v>
       </c>
       <c r="I11">
-        <v>-0.019</v>
+        <v>-1.9E-2</v>
       </c>
       <c r="J11">
-        <v>0.006</v>
+        <v>6.0000000000000001E-3</v>
       </c>
       <c r="K11">
         <v>-0.02</v>
       </c>
       <c r="L11">
-        <v>0.047</v>
+        <v>4.7E-2</v>
       </c>
       <c r="M11">
-        <v>-0.005</v>
+        <v>-5.0000000000000001E-3</v>
+      </c>
+      <c r="O11">
+        <f t="shared" si="1"/>
+        <v>0.106</v>
+      </c>
+      <c r="P11">
+        <f t="shared" si="2"/>
+        <v>1.6E-2</v>
+      </c>
+      <c r="Q11">
+        <f t="shared" si="3"/>
+        <v>0.53800000000000003</v>
+      </c>
+      <c r="R11">
+        <f t="shared" si="4"/>
+        <v>0.125</v>
+      </c>
+      <c r="S11">
+        <f t="shared" si="5"/>
+        <v>0.17100000000000001</v>
+      </c>
+      <c r="T11">
+        <f t="shared" si="6"/>
+        <v>0.80300000000000005</v>
+      </c>
+      <c r="U11">
+        <f t="shared" si="7"/>
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="V11">
+        <f t="shared" si="8"/>
+        <v>1.9E-2</v>
+      </c>
+      <c r="W11">
+        <f t="shared" si="9"/>
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="X11">
+        <f t="shared" si="10"/>
+        <v>0.02</v>
+      </c>
+      <c r="Y11">
+        <f t="shared" si="11"/>
+        <v>4.7E-2</v>
+      </c>
+      <c r="Z11">
+        <f t="shared" si="12"/>
+        <v>5.0000000000000001E-3</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="O2:Z2">
+    <cfRule type="top10" priority="22" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O2:Z2">
+    <cfRule type="top10" dxfId="10" priority="21" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O3:Z3">
+    <cfRule type="top10" priority="18" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O3:Z3">
+    <cfRule type="top10" dxfId="8" priority="17" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O4:Z4">
+    <cfRule type="top10" priority="16" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O4:Z4">
+    <cfRule type="top10" dxfId="7" priority="15" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O5:Z5">
+    <cfRule type="top10" priority="14" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O5:Z5">
+    <cfRule type="top10" dxfId="6" priority="13" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O6:Z6">
+    <cfRule type="top10" priority="12" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O6:Z6">
+    <cfRule type="top10" dxfId="5" priority="11" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O7:Z7">
+    <cfRule type="top10" priority="10" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O7:Z7">
+    <cfRule type="top10" dxfId="4" priority="9" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O8:Z8">
+    <cfRule type="top10" priority="8" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O8:Z8">
+    <cfRule type="top10" dxfId="3" priority="7" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O9:Z9">
+    <cfRule type="top10" priority="6" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O9:Z9">
+    <cfRule type="top10" dxfId="2" priority="5" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O10:Z10">
+    <cfRule type="top10" priority="4" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O10:Z10">
+    <cfRule type="top10" dxfId="1" priority="3" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O11:Z11">
+    <cfRule type="top10" priority="2" rank="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="O11:Z11">
+    <cfRule type="top10" dxfId="0" priority="1" rank="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E14"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>27</v>
       </c>
@@ -1841,7 +2520,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -1858,7 +2537,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -1875,7 +2554,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -1892,7 +2571,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="5" spans="1:5">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -1903,13 +2582,13 @@
         <v>13</v>
       </c>
       <c r="D5">
-        <v>-0.57</v>
+        <v>-0.56999999999999995</v>
       </c>
       <c r="E5" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="6" spans="1:5">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -1926,7 +2605,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:5">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1937,13 +2616,13 @@
         <v>10</v>
       </c>
       <c r="D7">
-        <v>0.759</v>
+        <v>0.75900000000000001</v>
       </c>
       <c r="E7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="8" spans="1:5">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1954,13 +2633,13 @@
         <v>12</v>
       </c>
       <c r="D8">
-        <v>-0.611</v>
+        <v>-0.61099999999999999</v>
       </c>
       <c r="E8" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="9" spans="1:5">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1971,13 +2650,13 @@
         <v>8</v>
       </c>
       <c r="D9">
-        <v>0.535</v>
+        <v>0.53500000000000003</v>
       </c>
       <c r="E9" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="10" spans="1:5">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1988,13 +2667,13 @@
         <v>3</v>
       </c>
       <c r="D10">
-        <v>-0.598</v>
+        <v>-0.59799999999999998</v>
       </c>
       <c r="E10" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="11" spans="1:5">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -2005,13 +2684,13 @@
         <v>7</v>
       </c>
       <c r="D11">
-        <v>0.803</v>
+        <v>0.80300000000000005</v>
       </c>
       <c r="E11" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="12" spans="1:5">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -2022,13 +2701,13 @@
         <v>4</v>
       </c>
       <c r="D12">
-        <v>0.674</v>
+        <v>0.67400000000000004</v>
       </c>
       <c r="E12" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -2039,13 +2718,13 @@
         <v>2</v>
       </c>
       <c r="D13">
-        <v>0.717</v>
+        <v>0.71699999999999997</v>
       </c>
       <c r="E13" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="14" spans="1:5">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -2056,7 +2735,7 @@
         <v>5</v>
       </c>
       <c r="D14">
-        <v>-0.5590000000000001</v>
+        <v>-0.55900000000000005</v>
       </c>
       <c r="E14" t="s">
         <v>44</v>
@@ -2068,14 +2747,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B1" s="1" t="s">
         <v>45</v>
       </c>
@@ -2083,7 +2762,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>5</v>
       </c>
@@ -2091,10 +2770,10 @@
         <v>7</v>
       </c>
       <c r="C2">
-        <v>0.535</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3">
+        <v>0.53500000000000003</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>3</v>
       </c>
@@ -2105,7 +2784,7 @@
         <v>0.151</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>4</v>
       </c>
@@ -2113,10 +2792,10 @@
         <v>6</v>
       </c>
       <c r="C4">
-        <v>0.095</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3">
+        <v>9.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>9</v>
       </c>
@@ -2124,10 +2803,10 @@
         <v>11</v>
       </c>
       <c r="C5">
-        <v>0.07000000000000001</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3">
+        <v>7.0000000000000007E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -2135,10 +2814,10 @@
         <v>3</v>
       </c>
       <c r="C6">
-        <v>0.037</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3">
+        <v>3.6999999999999998E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>10</v>
       </c>
@@ -2146,10 +2825,10 @@
         <v>12</v>
       </c>
       <c r="C7">
-        <v>0.031</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3">
+        <v>3.1E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -2157,10 +2836,10 @@
         <v>8</v>
       </c>
       <c r="C8">
-        <v>0.027</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3">
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>0</v>
       </c>
@@ -2168,10 +2847,10 @@
         <v>2</v>
       </c>
       <c r="C9">
-        <v>0.019</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
+        <v>1.9E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -2179,10 +2858,10 @@
         <v>10</v>
       </c>
       <c r="C10">
-        <v>0.019</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3">
+        <v>1.9E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>11</v>
       </c>
@@ -2190,10 +2869,10 @@
         <v>13</v>
       </c>
       <c r="C11">
-        <v>0.016</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3">
+        <v>1.6E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>2</v>
       </c>
@@ -2204,7 +2883,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>7</v>
       </c>

</xml_diff>